<commit_message>
Made final versions of database
</commit_message>
<xml_diff>
--- a/Documents/Database Schemas/Database Schema (4th Edit).xlsx
+++ b/Documents/Database Schemas/Database Schema (4th Edit).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnr\Documents\Coding\Web-Development-Project\Documents\Database Schemas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnr\OneDrive\Documents\Coding\Web-Development-Project\Documents\Database Schemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="112">
   <si>
     <t>Users</t>
   </si>
@@ -220,9 +220,6 @@
     <t>Banner</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>WRONG_SUBJECT</t>
   </si>
   <si>
@@ -326,6 +323,39 @@
   </si>
   <si>
     <t>Law</t>
+  </si>
+  <si>
+    <t>Claimant_Review</t>
+  </si>
+  <si>
+    <t>blah blah</t>
+  </si>
+  <si>
+    <t>Blah x3</t>
+  </si>
+  <si>
+    <t>Blah x4</t>
+  </si>
+  <si>
+    <t>Blah x5</t>
+  </si>
+  <si>
+    <t>Blah x6</t>
+  </si>
+  <si>
+    <t>Date_Banned</t>
+  </si>
+  <si>
+    <t>Ban_Desc</t>
+  </si>
+  <si>
+    <t>Spamming task stream</t>
+  </si>
+  <si>
+    <t>Creating inappropriate content</t>
+  </si>
+  <si>
+    <t>Blah x2</t>
   </si>
 </sst>
 </file>
@@ -706,7 +736,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -722,17 +752,6 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -745,6 +764,15 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -789,7 +817,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="3" applyBorder="1"/>
@@ -810,12 +837,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
@@ -1160,10 +1188,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N61" sqref="N61"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,27 +1204,27 @@
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="39"/>
-      <c r="B1" s="40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="40"/>
-    </row>
-    <row r="3" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="38"/>
+      <c r="B1" s="39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="40"/>
+      <c r="B2" s="39"/>
+    </row>
+    <row r="3" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
@@ -1219,7 +1247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>15167798</v>
       </c>
@@ -1229,7 +1257,7 @@
       <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="6">
@@ -1242,7 +1270,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>15159973</v>
       </c>
@@ -1252,7 +1280,7 @@
       <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="36" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="7">
@@ -1265,7 +1293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>15160513</v>
       </c>
@@ -1275,7 +1303,7 @@
       <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="36" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="7">
@@ -1288,7 +1316,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>15162788</v>
       </c>
@@ -1298,7 +1326,7 @@
       <c r="C8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="37" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="8">
@@ -1311,23 +1339,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="52"/>
+      <c r="C10" s="51"/>
       <c r="F10" s="31"/>
     </row>
-    <row r="11" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="53" t="s">
-        <v>92</v>
+      <c r="C11" s="52" t="s">
+        <v>91</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>26</v>
@@ -1347,8 +1375,11 @@
       <c r="I11" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1365,7 +1396,7 @@
         <v>41</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G12" s="6">
         <v>3</v>
@@ -1373,11 +1404,14 @@
       <c r="H12" s="6">
         <v>2500</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="53" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
@@ -1394,7 +1428,7 @@
         <v>42</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" s="7">
         <v>2</v>
@@ -1402,11 +1436,14 @@
       <c r="H13" s="7">
         <v>1000</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
@@ -1423,7 +1460,7 @@
         <v>43</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G14" s="7">
         <v>3</v>
@@ -1431,11 +1468,14 @@
       <c r="H14" s="7">
         <v>2750</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
@@ -1452,7 +1492,7 @@
         <v>42</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G15" s="7">
         <v>3</v>
@@ -1460,37 +1500,43 @@
       <c r="H15" s="7">
         <v>3000</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J15" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="35">
+        <v>69</v>
+      </c>
+      <c r="B16" s="34">
         <v>15167798</v>
       </c>
       <c r="C16" s="22">
         <v>42887</v>
       </c>
-      <c r="D16" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="35" t="s">
+      <c r="D16" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="35">
+      <c r="G16" s="34">
         <v>3</v>
       </c>
-      <c r="H16" s="35">
+      <c r="H16" s="34">
         <v>2800</v>
       </c>
       <c r="I16" s="34" t="s">
         <v>46</v>
+      </c>
+      <c r="J16" s="58" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1506,7 +1552,7 @@
     </row>
     <row r="18" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
@@ -1517,11 +1563,11 @@
       <c r="I18" s="29"/>
     </row>
     <row r="19" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="57" t="s">
-        <v>81</v>
+      <c r="B19" s="54" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1555,10 +1601,11 @@
       <c r="B23" s="1">
         <v>4</v>
       </c>
+      <c r="I23" s="59"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
@@ -1568,28 +1615,28 @@
     <row r="25" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="47" t="s">
+      <c r="A27" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="48" t="s">
-        <v>96</v>
+      <c r="C27" s="47" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>1</v>
       </c>
-      <c r="B28" s="60" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="54">
+      <c r="B28" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="53">
         <v>111</v>
       </c>
     </row>
@@ -1597,8 +1644,8 @@
       <c r="A29" s="4">
         <v>2</v>
       </c>
-      <c r="B29" s="58" t="s">
-        <v>86</v>
+      <c r="B29" s="55" t="s">
+        <v>85</v>
       </c>
       <c r="C29" s="1">
         <v>222</v>
@@ -1608,8 +1655,8 @@
       <c r="A30" s="4">
         <v>3</v>
       </c>
-      <c r="B30" s="58" t="s">
-        <v>87</v>
+      <c r="B30" s="55" t="s">
+        <v>86</v>
       </c>
       <c r="C30" s="1">
         <v>333</v>
@@ -1619,8 +1666,8 @@
       <c r="A31" s="5">
         <v>4</v>
       </c>
-      <c r="B31" s="59" t="s">
-        <v>88</v>
+      <c r="B31" s="56" t="s">
+        <v>87</v>
       </c>
       <c r="C31" s="2">
         <v>444</v>
@@ -1631,63 +1678,63 @@
     </row>
     <row r="33" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="46" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="47" t="s">
+    <row r="35" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>111</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="55">
-        <v>111</v>
-      </c>
-      <c r="B35" s="1" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>222</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>333</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="55">
-        <v>222</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="55">
-        <v>333</v>
-      </c>
-      <c r="B37" s="1" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>444</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>555</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="55">
-        <v>444</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="55">
-        <v>555</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
     <row r="40" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="56">
+      <c r="A40" s="5">
         <v>666</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1721,7 +1768,7 @@
         <v>15162788</v>
       </c>
       <c r="C44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>52</v>
@@ -1738,7 +1785,7 @@
         <v>15160513</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>53</v>
@@ -1755,7 +1802,7 @@
         <v>15160513</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>52</v>
@@ -1772,7 +1819,7 @@
         <v>15159973</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>53</v>
@@ -1789,7 +1836,7 @@
         <v>15162788</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>52</v>
@@ -1864,8 +1911,8 @@
       <c r="A57" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F57" s="42" t="s">
-        <v>76</v>
+      <c r="F57" s="41" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1878,11 +1925,11 @@
       <c r="C58" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D58" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="F58" s="43" t="s">
-        <v>80</v>
+      <c r="D58" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="F58" s="42" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1892,13 +1939,13 @@
       <c r="B59" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C59" s="49">
+      <c r="C59" s="48">
         <v>15162788</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F59" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="F59" s="43" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1909,14 +1956,14 @@
       <c r="B60" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C60" s="50">
+      <c r="C60" s="49">
         <v>15160513</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F60" s="44" t="s">
-        <v>77</v>
+        <v>89</v>
+      </c>
+      <c r="F60" s="43" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1926,14 +1973,14 @@
       <c r="B61" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C61" s="50">
+      <c r="C61" s="49">
         <v>15159973</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F61" s="44" t="s">
-        <v>78</v>
+        <v>90</v>
+      </c>
+      <c r="F61" s="43" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1943,18 +1990,18 @@
       <c r="B62" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="51">
+      <c r="C62" s="50">
         <v>15167798</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F62" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="F62" s="43" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F63" s="45" t="s">
+      <c r="F63" s="44" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1963,62 +2010,77 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>65</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>15167798</v>
       </c>
       <c r="B66" s="7">
         <v>15162788</v>
       </c>
-      <c r="C66" s="17">
+      <c r="C66" s="20">
         <v>42826</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="23">
         <v>15162788</v>
       </c>
       <c r="B67" s="7">
         <v>15160513</v>
       </c>
-      <c r="C67" s="18">
+      <c r="C67" s="21">
         <v>42827</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="25">
         <v>15160513</v>
       </c>
       <c r="B68" s="7">
         <v>15159973</v>
       </c>
-      <c r="C68" s="18">
+      <c r="C68" s="21">
         <v>42828</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D68" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="24">
         <v>15159973</v>
       </c>
       <c r="B69" s="8">
         <v>15162788</v>
       </c>
-      <c r="C69" s="19">
+      <c r="C69" s="22">
         <v>42829</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="D69" s="60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1"/>

</xml_diff>